<commit_message>
improved the text on the forms
</commit_message>
<xml_diff>
--- a/forms/contact/subcounty_hospital-create.xlsx
+++ b/forms/contact/subcounty_hospital-create.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -1138,7 +1138,7 @@
     <t xml:space="preserve">default_language</t>
   </si>
   <si>
-    <t xml:space="preserve">New PLACE_NAME</t>
+    <t xml:space="preserve">New Sub County</t>
   </si>
   <si>
     <t xml:space="preserve">contact:PLACE_TYPE:create</t>
@@ -1544,7 +1544,7 @@
       <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.71"/>
@@ -5743,8 +5743,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="75" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="75" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -5759,11 +5759,11 @@
   </sheetPr>
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29"/>
@@ -6418,8 +6418,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="75" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="75" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -6434,11 +6434,11 @@
   </sheetPr>
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.71"/>
@@ -6478,7 +6478,7 @@
       </c>
       <c r="C2" s="37" t="str">
         <f aca="true">TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2023-07-10  13-29</v>
+        <v>2023-07-13  18-42</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>372</v>
@@ -7487,8 +7487,8 @@
     <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="75" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="75" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>